<commit_message>
updated files with strain names
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_fullrun_hbrown_12.04.19.xlsx
+++ b/fastqFiles/fastq_fullrun_hbrown_12.04.19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FCB248-7AF7-7C41-BDA1-D0EB54B063CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A627A7-E55B-DF42-870B-8768B3D659EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33580" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33580" windowHeight="16840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -590,7 +590,7 @@
   <dimension ref="A1:Z41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>